<commit_message>
Uren planning update, and doxygen config added
</commit_message>
<xml_diff>
--- a/Docs/planning/Urenplanning en verantwoording themaopdracht Devices.xlsx
+++ b/Docs/planning/Urenplanning en verantwoording themaopdracht Devices.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="56">
   <si>
     <t>lesweek</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Uitschrijven schietknop</t>
   </si>
   <si>
-    <t>Uitschrijven Score aan console geven</t>
-  </si>
-  <si>
     <t>Uitschrijven keypad</t>
   </si>
   <si>
@@ -187,6 +184,12 @@
   </si>
   <si>
     <t>Game controller</t>
+  </si>
+  <si>
+    <t>VERVALLEN</t>
+  </si>
+  <si>
+    <t>documenteren</t>
   </si>
 </sst>
 </file>
@@ -509,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -632,15 +635,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -702,12 +696,36 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -745,7 +763,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -856,9 +873,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$22:$C$55</c:f>
+              <c:f>Sheet1!$A$22:$C$56</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Besprekingen met begeleider</c:v>
@@ -903,13 +920,13 @@
                     <c:v>Debuggen</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>Uitschrijven Score aan console geven</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>Testen</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>Debuggen</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="17">
                     <c:v>Uitschrijven game starter</c:v>
@@ -957,9 +974,12 @@
                     <c:v>debuggen</c:v>
                   </c:pt>
                   <c:pt idx="32">
+                    <c:v>documenteren</c:v>
+                  </c:pt>
+                  <c:pt idx="33">
                     <c:v>Besprekingen met begeleider</c:v>
                   </c:pt>
-                  <c:pt idx="33">
+                  <c:pt idx="34">
                     <c:v>weektotaal</c:v>
                   </c:pt>
                 </c:lvl>
@@ -967,10 +987,28 @@
                   <c:pt idx="0">
                     <c:v>24,27-okt</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="2">
                     <c:v>Projectweek 3</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -978,10 +1016,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$22:$D$55</c:f>
+              <c:f>Sheet1!$D$22:$D$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1004,7 +1042,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1025,7 +1063,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -1070,19 +1108,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="33">
-                  <c:v>52</c:v>
+                <c:pt idx="34">
+                  <c:v>55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1163,9 +1204,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$22:$C$55</c:f>
+              <c:f>Sheet1!$A$22:$C$56</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Besprekingen met begeleider</c:v>
@@ -1210,13 +1251,13 @@
                     <c:v>Debuggen</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>Uitschrijven Score aan console geven</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>Testen</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>Debuggen</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="17">
                     <c:v>Uitschrijven game starter</c:v>
@@ -1264,9 +1305,12 @@
                     <c:v>debuggen</c:v>
                   </c:pt>
                   <c:pt idx="32">
+                    <c:v>documenteren</c:v>
+                  </c:pt>
+                  <c:pt idx="33">
                     <c:v>Besprekingen met begeleider</c:v>
                   </c:pt>
-                  <c:pt idx="33">
+                  <c:pt idx="34">
                     <c:v>weektotaal</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1274,10 +1318,28 @@
                   <c:pt idx="0">
                     <c:v>24,27-okt</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="2">
                     <c:v>Projectweek 3</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1285,18 +1347,87 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$22:$E$55</c:f>
+              <c:f>Sheet1!$E$22:$E$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>27</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4</c:v>
+                </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1376,9 +1507,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$22:$C$55</c:f>
+              <c:f>Sheet1!$A$22:$C$56</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Besprekingen met begeleider</c:v>
@@ -1423,13 +1554,13 @@
                     <c:v>Debuggen</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>Uitschrijven Score aan console geven</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>Testen</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>Debuggen</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="17">
                     <c:v>Uitschrijven game starter</c:v>
@@ -1477,9 +1608,12 @@
                     <c:v>debuggen</c:v>
                   </c:pt>
                   <c:pt idx="32">
+                    <c:v>documenteren</c:v>
+                  </c:pt>
+                  <c:pt idx="33">
                     <c:v>Besprekingen met begeleider</c:v>
                   </c:pt>
-                  <c:pt idx="33">
+                  <c:pt idx="34">
                     <c:v>weektotaal</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1487,10 +1621,28 @@
                   <c:pt idx="0">
                     <c:v>24,27-okt</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="2">
                     <c:v>Projectweek 3</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1498,10 +1650,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$22:$F$55</c:f>
+              <c:f>Sheet1!$F$22:$F$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1509,7 +1661,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
@@ -1524,7 +1676,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1590,18 +1742,21 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>54</c:v>
                 </c:pt>
               </c:numCache>
@@ -1621,13 +1776,13 @@
 uren</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2</c:v>
@@ -1654,7 +1809,7 @@
                   <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>-</c:v>
@@ -1683,9 +1838,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$22:$C$55</c:f>
+              <c:f>Sheet1!$A$22:$C$56</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Besprekingen met begeleider</c:v>
@@ -1730,13 +1885,13 @@
                     <c:v>Debuggen</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>Uitschrijven Score aan console geven</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>Testen</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>Debuggen</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="17">
                     <c:v>Uitschrijven game starter</c:v>
@@ -1784,9 +1939,12 @@
                     <c:v>debuggen</c:v>
                   </c:pt>
                   <c:pt idx="32">
+                    <c:v>documenteren</c:v>
+                  </c:pt>
+                  <c:pt idx="33">
                     <c:v>Besprekingen met begeleider</c:v>
                   </c:pt>
-                  <c:pt idx="33">
+                  <c:pt idx="34">
                     <c:v>weektotaal</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1794,10 +1952,28 @@
                   <c:pt idx="0">
                     <c:v>24,27-okt</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="2">
                     <c:v>Projectweek 3</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1805,18 +1981,105 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$22:$G$55</c:f>
+              <c:f>Sheet1!$G$22:$G$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23</c:v>
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1896,9 +2159,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$22:$C$55</c:f>
+              <c:f>Sheet1!$A$22:$C$56</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Besprekingen met begeleider</c:v>
@@ -1943,13 +2206,13 @@
                     <c:v>Debuggen</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>Uitschrijven Score aan console geven</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>Testen</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>Debuggen</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="17">
                     <c:v>Uitschrijven game starter</c:v>
@@ -1997,9 +2260,12 @@
                     <c:v>debuggen</c:v>
                   </c:pt>
                   <c:pt idx="32">
+                    <c:v>documenteren</c:v>
+                  </c:pt>
+                  <c:pt idx="33">
                     <c:v>Besprekingen met begeleider</c:v>
                   </c:pt>
-                  <c:pt idx="33">
+                  <c:pt idx="34">
                     <c:v>weektotaal</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2007,10 +2273,28 @@
                   <c:pt idx="0">
                     <c:v>24,27-okt</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="2">
                     <c:v>Projectweek 3</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -2018,10 +2302,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$22:$H$55</c:f>
+              <c:f>Sheet1!$H$22:$H$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2029,7 +2313,7 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2</c:v>
@@ -2092,7 +2376,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0</c:v>
@@ -2110,19 +2394,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="33">
-                  <c:v>52</c:v>
+                <c:pt idx="34">
+                  <c:v>56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2144,7 +2431,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>6</c:v>
@@ -2203,9 +2490,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$22:$C$55</c:f>
+              <c:f>Sheet1!$A$22:$C$56</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Besprekingen met begeleider</c:v>
@@ -2250,13 +2537,13 @@
                     <c:v>Debuggen</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>Uitschrijven Score aan console geven</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>Testen</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>Debuggen</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="17">
                     <c:v>Uitschrijven game starter</c:v>
@@ -2304,9 +2591,12 @@
                     <c:v>debuggen</c:v>
                   </c:pt>
                   <c:pt idx="32">
+                    <c:v>documenteren</c:v>
+                  </c:pt>
+                  <c:pt idx="33">
                     <c:v>Besprekingen met begeleider</c:v>
                   </c:pt>
-                  <c:pt idx="33">
+                  <c:pt idx="34">
                     <c:v>weektotaal</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2314,10 +2604,28 @@
                   <c:pt idx="0">
                     <c:v>24,27-okt</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="2">
                     <c:v>Projectweek 3</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -2325,18 +2633,105 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$22:$I$55</c:f>
+              <c:f>Sheet1!$I$22:$I$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2418,9 +2813,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$22:$C$55</c:f>
+              <c:f>Sheet1!$A$22:$C$56</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Besprekingen met begeleider</c:v>
@@ -2465,13 +2860,13 @@
                     <c:v>Debuggen</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>Uitschrijven Score aan console geven</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>Testen</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>Debuggen</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="17">
                     <c:v>Uitschrijven game starter</c:v>
@@ -2519,9 +2914,12 @@
                     <c:v>debuggen</c:v>
                   </c:pt>
                   <c:pt idx="32">
+                    <c:v>documenteren</c:v>
+                  </c:pt>
+                  <c:pt idx="33">
                     <c:v>Besprekingen met begeleider</c:v>
                   </c:pt>
-                  <c:pt idx="33">
+                  <c:pt idx="34">
                     <c:v>weektotaal</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2529,10 +2927,28 @@
                   <c:pt idx="0">
                     <c:v>24,27-okt</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="2">
                     <c:v>Projectweek 3</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -2540,10 +2956,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$22:$J$55</c:f>
+              <c:f>Sheet1!$J$22:$J$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2587,7 +3003,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -2632,19 +3048,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="33">
-                  <c:v>48</c:v>
+                <c:pt idx="34">
+                  <c:v>53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2663,10 +3082,10 @@
 uren</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>6</c:v>
@@ -2727,9 +3146,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$22:$C$55</c:f>
+              <c:f>Sheet1!$A$22:$C$56</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Besprekingen met begeleider</c:v>
@@ -2774,13 +3193,13 @@
                     <c:v>Debuggen</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>Uitschrijven Score aan console geven</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>Testen</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>Debuggen</c:v>
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                   <c:pt idx="17">
                     <c:v>Uitschrijven game starter</c:v>
@@ -2828,9 +3247,12 @@
                     <c:v>debuggen</c:v>
                   </c:pt>
                   <c:pt idx="32">
+                    <c:v>documenteren</c:v>
+                  </c:pt>
+                  <c:pt idx="33">
                     <c:v>Besprekingen met begeleider</c:v>
                   </c:pt>
-                  <c:pt idx="33">
+                  <c:pt idx="34">
                     <c:v>weektotaal</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2838,10 +3260,28 @@
                   <c:pt idx="0">
                     <c:v>24,27-okt</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="2">
                     <c:v>Projectweek 3</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>VERVALLEN</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>VERVALLEN</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -2849,18 +3289,78 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$22:$K$55</c:f>
+              <c:f>Sheet1!$K$22:$K$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2876,11 +3376,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="441058496"/>
-        <c:axId val="441059280"/>
+        <c:axId val="372853408"/>
+        <c:axId val="372853800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="441058496"/>
+        <c:axId val="372853408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2923,7 +3423,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="441059280"/>
+        <c:crossAx val="372853800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2931,7 +3431,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="441059280"/>
+        <c:axId val="372853800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2982,7 +3482,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="441058496"/>
+        <c:crossAx val="372853408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2996,7 +3496,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3926,10 +4425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L136"/>
+  <dimension ref="A1:L137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3973,22 +4472,22 @@
       <c r="A3" s="15"/>
       <c r="B3" s="20"/>
       <c r="C3" s="21"/>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="56" t="s">
+      <c r="E3" s="89"/>
+      <c r="F3" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56" t="s">
+      <c r="G3" s="90"/>
+      <c r="H3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56" t="s">
+      <c r="I3" s="90"/>
+      <c r="J3" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="56"/>
+      <c r="K3" s="90"/>
       <c r="L3" s="23"/>
     </row>
     <row r="5" spans="1:12" s="29" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4029,10 +4528,10 @@
     <row r="6" spans="1:12" s="29" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="35"/>
       <c r="B6" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="38">
         <v>2</v>
@@ -4044,7 +4543,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H6" s="40">
         <v>2</v>
@@ -4056,7 +4555,7 @@
         <v>2</v>
       </c>
       <c r="K6" s="41">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="29" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -4064,10 +4563,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="38">
         <v>1</v>
@@ -4085,22 +4584,22 @@
         <v>1</v>
       </c>
       <c r="I7" s="40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" s="41">
         <v>1</v>
       </c>
       <c r="K7" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="29" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="53"/>
       <c r="B8" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="36" t="s">
         <v>49</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>50</v>
       </c>
       <c r="D8" s="38">
         <v>6</v>
@@ -4112,7 +4611,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="40">
         <v>6</v>
@@ -4133,7 +4632,7 @@
         <v>42667</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="38">
         <v>2</v>
@@ -4162,7 +4661,7 @@
     </row>
     <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>20</v>
@@ -4261,7 +4760,7 @@
     <row r="13" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>21</v>
@@ -4360,7 +4859,7 @@
     <row r="16" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>27</v>
@@ -4408,7 +4907,7 @@
         <v>6</v>
       </c>
       <c r="G17" s="43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17" s="44" t="s">
         <v>6</v>
@@ -4459,7 +4958,7 @@
     <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>30</v>
@@ -4523,108 +5022,108 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="57"/>
-      <c r="B21" s="58">
+      <c r="A21" s="54"/>
+      <c r="B21" s="55">
         <v>42670</v>
       </c>
       <c r="C21" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="59" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="59" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="60" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="60" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="61">
+      <c r="D21" s="56" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="56" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="58">
         <v>4</v>
       </c>
-      <c r="I21" s="61">
+      <c r="I21" s="58">
         <v>4</v>
       </c>
-      <c r="J21" s="62" t="s">
-        <v>6</v>
-      </c>
-      <c r="K21" s="62" t="s">
+      <c r="J21" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="K21" s="59" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="33"/>
-      <c r="B22" s="69" t="s">
-        <v>52</v>
+      <c r="B22" s="66" t="s">
+        <v>51</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="65" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="65">
+        <v>50</v>
+      </c>
+      <c r="D22" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="62">
         <v>2</v>
       </c>
-      <c r="F22" s="66" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" s="66">
+      <c r="F22" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="63">
         <v>2</v>
       </c>
-      <c r="H22" s="67" t="s">
-        <v>6</v>
-      </c>
-      <c r="I22" s="67">
+      <c r="H22" s="64" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" s="64">
         <v>2</v>
       </c>
-      <c r="J22" s="68" t="s">
-        <v>6</v>
-      </c>
-      <c r="K22" s="68">
+      <c r="J22" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="K22" s="65">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="63"/>
-      <c r="B23" s="63"/>
+      <c r="A23" s="60"/>
+      <c r="B23" s="60"/>
       <c r="C23" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="64">
+      <c r="D23" s="61">
         <f>SUM(D6:D22)</f>
         <v>22</v>
       </c>
-      <c r="E23" s="64">
+      <c r="E23" s="61">
         <f>SUM(E6:E22)</f>
         <v>27</v>
       </c>
-      <c r="F23" s="64">
+      <c r="F23" s="61">
         <f>SUM(F6:F22)</f>
         <v>20</v>
       </c>
-      <c r="G23" s="64">
+      <c r="G23" s="61">
         <f>SUM(G6:G22)</f>
-        <v>23</v>
-      </c>
-      <c r="H23" s="64">
+        <v>26</v>
+      </c>
+      <c r="H23" s="61">
         <f>SUM(H7:H22)</f>
         <v>19</v>
       </c>
-      <c r="I23" s="64">
+      <c r="I23" s="61">
         <f>SUM(I6:I22)</f>
-        <v>23</v>
-      </c>
-      <c r="J23" s="64">
+        <v>24</v>
+      </c>
+      <c r="J23" s="61">
         <f>SUM(J6:J22)</f>
         <v>22</v>
       </c>
-      <c r="K23" s="64">
+      <c r="K23" s="61">
         <f>SUM(K6:K22)</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4632,355 +5131,487 @@
         <v>9</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="70" t="s">
-        <v>53</v>
+      <c r="C24" s="67" t="s">
+        <v>52</v>
       </c>
       <c r="D24" s="42">
         <v>16</v>
       </c>
-      <c r="E24" s="42"/>
-      <c r="F24" s="43">
-        <v>8</v>
-      </c>
-      <c r="G24" s="43"/>
-      <c r="H24" s="44">
-        <v>2</v>
-      </c>
-      <c r="I24" s="44"/>
+      <c r="E24" s="42">
+        <v>22</v>
+      </c>
+      <c r="F24" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="44">
+        <v>4</v>
+      </c>
       <c r="J24" s="45">
         <v>10</v>
       </c>
-      <c r="K24" s="45"/>
+      <c r="K24" s="45">
+        <v>20</v>
+      </c>
     </row>
     <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="30"/>
-      <c r="C25" s="75" t="s">
-        <v>39</v>
+      <c r="C25" s="72" t="s">
+        <v>38</v>
       </c>
       <c r="D25" s="42">
         <v>1</v>
       </c>
-      <c r="E25" s="42"/>
+      <c r="E25" s="42">
+        <v>6</v>
+      </c>
       <c r="F25" s="43">
         <v>1</v>
       </c>
-      <c r="G25" s="43"/>
+      <c r="G25" s="43">
+        <v>6</v>
+      </c>
       <c r="H25" s="44">
         <v>2</v>
       </c>
-      <c r="I25" s="44"/>
+      <c r="I25" s="44">
+        <v>6</v>
+      </c>
       <c r="J25" s="45">
         <v>2</v>
       </c>
-      <c r="K25" s="45"/>
+      <c r="K25" s="45">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="B26" s="30"/>
-      <c r="C26" s="80" t="s">
-        <v>41</v>
+      <c r="C26" s="77" t="s">
+        <v>40</v>
       </c>
       <c r="D26" s="42">
         <v>1</v>
       </c>
-      <c r="E26" s="42"/>
+      <c r="E26" s="42">
+        <v>10</v>
+      </c>
       <c r="F26" s="43">
         <v>1</v>
       </c>
-      <c r="G26" s="43"/>
+      <c r="G26" s="43">
+        <v>10</v>
+      </c>
       <c r="H26" s="44">
         <v>2</v>
       </c>
-      <c r="I26" s="44"/>
+      <c r="I26" s="44">
+        <v>10</v>
+      </c>
       <c r="J26" s="45">
         <v>2</v>
       </c>
-      <c r="K26" s="45"/>
+      <c r="K26" s="45">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="30"/>
-      <c r="C27" s="89" t="s">
-        <v>54</v>
+      <c r="C27" s="85" t="s">
+        <v>53</v>
       </c>
       <c r="D27" s="42">
         <v>5</v>
       </c>
-      <c r="E27" s="42"/>
+      <c r="E27" s="42">
+        <v>2</v>
+      </c>
       <c r="F27" s="43">
         <v>5</v>
       </c>
-      <c r="G27" s="43"/>
+      <c r="G27" s="43">
+        <v>2</v>
+      </c>
       <c r="H27" s="44">
         <v>5</v>
       </c>
-      <c r="I27" s="44"/>
+      <c r="I27" s="44">
+        <v>7</v>
+      </c>
       <c r="J27" s="45">
         <v>5</v>
       </c>
-      <c r="K27" s="45"/>
+      <c r="K27" s="45">
+        <v>4</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="30"/>
-      <c r="C28" s="90" t="s">
-        <v>39</v>
+      <c r="C28" s="86" t="s">
+        <v>38</v>
       </c>
       <c r="D28" s="42">
         <v>2</v>
       </c>
-      <c r="E28" s="42"/>
+      <c r="E28" s="42" t="s">
+        <v>6</v>
+      </c>
       <c r="F28" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G28" s="43"/>
+      <c r="G28" s="43" t="s">
+        <v>6</v>
+      </c>
       <c r="H28" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="I28" s="44"/>
+      <c r="I28" s="44">
+        <v>3</v>
+      </c>
       <c r="J28" s="45">
         <v>2</v>
       </c>
-      <c r="K28" s="88"/>
+      <c r="K28" s="45">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="30"/>
-      <c r="C29" s="91" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="42">
-        <v>2</v>
-      </c>
-      <c r="E29" s="42"/>
-      <c r="F29" s="43">
-        <v>2</v>
-      </c>
-      <c r="G29" s="43"/>
+      <c r="C29" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="43" t="s">
+        <v>6</v>
+      </c>
       <c r="H29" s="44">
         <v>2</v>
       </c>
-      <c r="I29" s="44"/>
+      <c r="I29" s="44">
+        <v>3</v>
+      </c>
       <c r="J29" s="45">
         <v>2</v>
       </c>
-      <c r="K29" s="45"/>
+      <c r="K29" s="45">
+        <v>3</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="34"/>
-      <c r="C30" s="71" t="s">
+      <c r="C30" s="68" t="s">
         <v>32</v>
       </c>
       <c r="D30" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="42"/>
+      <c r="E30" s="42">
+        <v>2</v>
+      </c>
       <c r="F30" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G30" s="43"/>
+      <c r="G30" s="43" t="s">
+        <v>6</v>
+      </c>
       <c r="H30" s="44">
         <v>5</v>
       </c>
-      <c r="I30" s="44"/>
+      <c r="I30" s="44">
+        <v>1</v>
+      </c>
       <c r="J30" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="K30" s="45"/>
+      <c r="K30" s="45" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="34"/>
-      <c r="C31" s="76" t="s">
-        <v>39</v>
+      <c r="C31" s="73" t="s">
+        <v>38</v>
       </c>
       <c r="D31" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="42"/>
+      <c r="E31" s="42">
+        <v>2</v>
+      </c>
       <c r="F31" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G31" s="43"/>
+      <c r="G31" s="43" t="s">
+        <v>6</v>
+      </c>
       <c r="H31" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="I31" s="44"/>
+      <c r="I31" s="44">
+        <v>1</v>
+      </c>
       <c r="J31" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="K31" s="45"/>
+      <c r="K31" s="45" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="32" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="B32" s="34"/>
-      <c r="C32" s="81" t="s">
-        <v>41</v>
+      <c r="C32" s="78" t="s">
+        <v>40</v>
       </c>
       <c r="D32" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="42"/>
+      <c r="E32" s="42">
+        <v>2</v>
+      </c>
       <c r="F32" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G32" s="43"/>
+      <c r="G32" s="43" t="s">
+        <v>6</v>
+      </c>
       <c r="H32" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="I32" s="44"/>
+      <c r="I32" s="44">
+        <v>1</v>
+      </c>
       <c r="J32" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="K32" s="45"/>
+      <c r="K32" s="45" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="33" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="34"/>
-      <c r="C33" s="71" t="s">
-        <v>34</v>
+      <c r="C33" s="68" t="s">
+        <v>33</v>
       </c>
       <c r="D33" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="42"/>
+      <c r="E33" s="42">
+        <v>2</v>
+      </c>
       <c r="F33" s="43">
         <v>5</v>
       </c>
-      <c r="G33" s="43"/>
+      <c r="G33" s="43">
+        <v>5</v>
+      </c>
       <c r="H33" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="I33" s="44"/>
+      <c r="I33" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="J33" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="K33" s="45"/>
+      <c r="K33" s="45" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="34" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
       <c r="B34" s="34"/>
-      <c r="C34" s="76" t="s">
-        <v>39</v>
+      <c r="C34" s="73" t="s">
+        <v>38</v>
       </c>
       <c r="D34" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="42"/>
+      <c r="E34" s="42">
+        <v>2</v>
+      </c>
       <c r="F34" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G34" s="43"/>
+      <c r="G34" s="43">
+        <v>2</v>
+      </c>
       <c r="H34" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="I34" s="44"/>
+      <c r="I34" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="J34" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="K34" s="45"/>
+      <c r="K34" s="45" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="35" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="34"/>
-      <c r="C35" s="81" t="s">
-        <v>41</v>
+      <c r="C35" s="78" t="s">
+        <v>40</v>
       </c>
       <c r="D35" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E35" s="42"/>
+      <c r="E35" s="42">
+        <v>2</v>
+      </c>
       <c r="F35" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G35" s="43"/>
+      <c r="G35" s="43">
+        <v>2</v>
+      </c>
       <c r="H35" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="I35" s="44"/>
+      <c r="I35" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="J35" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="K35" s="45"/>
+      <c r="K35" s="45" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="36" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="6"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="71" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" s="42">
-        <v>5</v>
-      </c>
-      <c r="E36" s="42"/>
-      <c r="F36" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="G36" s="43"/>
-      <c r="H36" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="I36" s="44"/>
-      <c r="J36" s="45">
-        <v>5</v>
-      </c>
-      <c r="K36" s="45"/>
+      <c r="A36" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="37" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="6"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="76" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" s="42"/>
-      <c r="F37" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="G37" s="43"/>
-      <c r="H37" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="I37" s="44"/>
-      <c r="J37" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="K37" s="45"/>
+      <c r="A37" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K37" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="38" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="6"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="81" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" s="42"/>
-      <c r="F38" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="G38" s="43"/>
-      <c r="H38" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="I38" s="44"/>
-      <c r="J38" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="K38" s="45"/>
+      <c r="A38" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J38" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K38" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="39" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="34"/>
-      <c r="C39" s="71" t="s">
-        <v>35</v>
-      </c>
-      <c r="D39" s="85" t="s">
+      <c r="C39" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="82" t="s">
         <v>6</v>
       </c>
       <c r="E39" s="42"/>
@@ -4991,7 +5622,9 @@
       <c r="H39" s="44">
         <v>2</v>
       </c>
-      <c r="I39" s="44"/>
+      <c r="I39" s="44">
+        <v>2</v>
+      </c>
       <c r="J39" s="45" t="s">
         <v>6</v>
       </c>
@@ -5000,8 +5633,8 @@
     <row r="40" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
       <c r="B40" s="34"/>
-      <c r="C40" s="75" t="s">
-        <v>39</v>
+      <c r="C40" s="72" t="s">
+        <v>38</v>
       </c>
       <c r="D40" s="42" t="s">
         <v>6</v>
@@ -5014,7 +5647,9 @@
       <c r="H40" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="I40" s="44"/>
+      <c r="I40" s="44">
+        <v>1</v>
+      </c>
       <c r="J40" s="45" t="s">
         <v>6</v>
       </c>
@@ -5023,8 +5658,8 @@
     <row r="41" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="B41" s="34"/>
-      <c r="C41" s="81" t="s">
-        <v>41</v>
+      <c r="C41" s="78" t="s">
+        <v>40</v>
       </c>
       <c r="D41" s="42" t="s">
         <v>6</v>
@@ -5037,7 +5672,9 @@
       <c r="H41" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="I41" s="44"/>
+      <c r="I41" s="44">
+        <v>1</v>
+      </c>
       <c r="J41" s="45" t="s">
         <v>6</v>
       </c>
@@ -5046,8 +5683,8 @@
     <row r="42" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
       <c r="B42" s="34"/>
-      <c r="C42" s="72" t="s">
-        <v>42</v>
+      <c r="C42" s="69" t="s">
+        <v>41</v>
       </c>
       <c r="D42" s="42" t="s">
         <v>6</v>
@@ -5056,11 +5693,15 @@
       <c r="F42" s="43">
         <v>6</v>
       </c>
-      <c r="G42" s="43"/>
+      <c r="G42" s="43">
+        <v>4</v>
+      </c>
       <c r="H42" s="44">
         <v>6</v>
       </c>
-      <c r="I42" s="44"/>
+      <c r="I42" s="44">
+        <v>4</v>
+      </c>
       <c r="J42" s="45" t="s">
         <v>6</v>
       </c>
@@ -5069,8 +5710,8 @@
     <row r="43" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="B43" s="34"/>
-      <c r="C43" s="77" t="s">
-        <v>39</v>
+      <c r="C43" s="74" t="s">
+        <v>38</v>
       </c>
       <c r="D43" s="42" t="s">
         <v>6</v>
@@ -5079,11 +5720,15 @@
       <c r="F43" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G43" s="43"/>
+      <c r="G43" s="43">
+        <v>2</v>
+      </c>
       <c r="H43" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="I43" s="44"/>
+      <c r="I43" s="44">
+        <v>2</v>
+      </c>
       <c r="J43" s="45" t="s">
         <v>6</v>
       </c>
@@ -5092,8 +5737,8 @@
     <row r="44" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
       <c r="B44" s="34"/>
-      <c r="C44" s="82" t="s">
-        <v>41</v>
+      <c r="C44" s="79" t="s">
+        <v>40</v>
       </c>
       <c r="D44" s="42" t="s">
         <v>6</v>
@@ -5102,11 +5747,15 @@
       <c r="F44" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G44" s="43"/>
+      <c r="G44" s="43">
+        <v>2</v>
+      </c>
       <c r="H44" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="I44" s="44"/>
+      <c r="I44" s="44">
+        <v>2</v>
+      </c>
       <c r="J44" s="45" t="s">
         <v>6</v>
       </c>
@@ -5114,21 +5763,27 @@
     </row>
     <row r="45" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="2"/>
-      <c r="C45" s="73" t="s">
-        <v>36</v>
+      <c r="C45" s="70" t="s">
+        <v>35</v>
       </c>
       <c r="D45" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E45" s="42"/>
+      <c r="E45" s="42">
+        <v>6</v>
+      </c>
       <c r="F45" s="43">
         <v>2</v>
       </c>
-      <c r="G45" s="43"/>
+      <c r="G45" s="43">
+        <v>6</v>
+      </c>
       <c r="H45" s="44">
-        <v>6</v>
-      </c>
-      <c r="I45" s="44"/>
+        <v>2</v>
+      </c>
+      <c r="I45" s="44">
+        <v>1</v>
+      </c>
       <c r="J45" s="45" t="s">
         <v>6</v>
       </c>
@@ -5137,21 +5792,27 @@
     <row r="46" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
       <c r="B46" s="2"/>
-      <c r="C46" s="78" t="s">
-        <v>39</v>
+      <c r="C46" s="75" t="s">
+        <v>38</v>
       </c>
       <c r="D46" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E46" s="42"/>
+      <c r="E46" s="42">
+        <v>2</v>
+      </c>
       <c r="F46" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G46" s="87"/>
+      <c r="G46" s="84">
+        <v>2</v>
+      </c>
       <c r="H46" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="I46" s="44"/>
+      <c r="I46" s="44">
+        <v>1</v>
+      </c>
       <c r="J46" s="45" t="s">
         <v>6</v>
       </c>
@@ -5160,21 +5821,27 @@
     <row r="47" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="7"/>
       <c r="B47" s="2"/>
-      <c r="C47" s="83" t="s">
-        <v>41</v>
+      <c r="C47" s="80" t="s">
+        <v>40</v>
       </c>
       <c r="D47" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E47" s="42"/>
+      <c r="E47" s="42">
+        <v>2</v>
+      </c>
       <c r="F47" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G47" s="43"/>
+      <c r="G47" s="43">
+        <v>2</v>
+      </c>
       <c r="H47" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="I47" s="44"/>
+      <c r="I47" s="44">
+        <v>1</v>
+      </c>
       <c r="J47" s="45" t="s">
         <v>6</v>
       </c>
@@ -5183,8 +5850,8 @@
     <row r="48" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
       <c r="B48" s="2"/>
-      <c r="C48" s="73" t="s">
-        <v>37</v>
+      <c r="C48" s="70" t="s">
+        <v>36</v>
       </c>
       <c r="D48" s="42" t="s">
         <v>6</v>
@@ -5193,7 +5860,9 @@
       <c r="F48" s="43">
         <v>4</v>
       </c>
-      <c r="G48" s="43"/>
+      <c r="G48" s="43">
+        <v>2</v>
+      </c>
       <c r="H48" s="44" t="s">
         <v>6</v>
       </c>
@@ -5206,8 +5875,8 @@
     <row r="49" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="2"/>
-      <c r="C49" s="79" t="s">
-        <v>39</v>
+      <c r="C49" s="76" t="s">
+        <v>38</v>
       </c>
       <c r="D49" s="42" t="s">
         <v>6</v>
@@ -5216,7 +5885,9 @@
       <c r="F49" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G49" s="43"/>
+      <c r="G49" s="43">
+        <v>2</v>
+      </c>
       <c r="H49" s="44" t="s">
         <v>6</v>
       </c>
@@ -5229,8 +5900,8 @@
     <row r="50" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6"/>
       <c r="B50" s="2"/>
-      <c r="C50" s="84" t="s">
-        <v>41</v>
+      <c r="C50" s="81" t="s">
+        <v>40</v>
       </c>
       <c r="D50" s="42" t="s">
         <v>6</v>
@@ -5239,7 +5910,9 @@
       <c r="F50" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G50" s="43"/>
+      <c r="G50" s="43">
+        <v>2</v>
+      </c>
       <c r="H50" s="44" t="s">
         <v>6</v>
       </c>
@@ -5252,250 +5925,276 @@
     <row r="51" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
       <c r="B51" s="2"/>
-      <c r="C51" s="74" t="s">
-        <v>38</v>
+      <c r="C51" s="71" t="s">
+        <v>37</v>
       </c>
       <c r="D51" s="42">
-        <v>4</v>
-      </c>
-      <c r="E51" s="42"/>
+        <v>8</v>
+      </c>
+      <c r="E51" s="42">
+        <v>8</v>
+      </c>
       <c r="F51" s="43">
-        <v>4</v>
-      </c>
-      <c r="G51" s="43"/>
+        <v>8</v>
+      </c>
+      <c r="G51" s="43">
+        <v>8</v>
+      </c>
       <c r="H51" s="44">
-        <v>4</v>
-      </c>
-      <c r="I51" s="44"/>
+        <v>8</v>
+      </c>
+      <c r="I51" s="44">
+        <v>8</v>
+      </c>
       <c r="J51" s="45">
-        <v>4</v>
-      </c>
-      <c r="K51" s="45"/>
+        <v>8</v>
+      </c>
+      <c r="K51" s="45">
+        <v>8</v>
+      </c>
     </row>
     <row r="52" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="6"/>
       <c r="B52" s="2"/>
-      <c r="C52" s="76" t="s">
-        <v>39</v>
+      <c r="C52" s="73" t="s">
+        <v>38</v>
       </c>
       <c r="D52" s="42">
         <v>8</v>
       </c>
-      <c r="E52" s="42"/>
+      <c r="E52" s="42">
+        <v>8</v>
+      </c>
       <c r="F52" s="43">
         <v>8</v>
       </c>
-      <c r="G52" s="43"/>
+      <c r="G52" s="43">
+        <v>8</v>
+      </c>
       <c r="H52" s="44">
         <v>8</v>
       </c>
-      <c r="I52" s="44"/>
+      <c r="I52" s="44">
+        <v>8</v>
+      </c>
       <c r="J52" s="45">
         <v>8</v>
       </c>
-      <c r="K52" s="45"/>
+      <c r="K52" s="45">
+        <v>8</v>
+      </c>
     </row>
     <row r="53" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="6"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="81" t="s">
-        <v>40</v>
-      </c>
-      <c r="D53" s="42">
-        <v>6</v>
-      </c>
-      <c r="E53" s="42"/>
-      <c r="F53" s="43">
-        <v>6</v>
-      </c>
-      <c r="G53" s="43"/>
-      <c r="H53" s="44">
-        <v>6</v>
-      </c>
-      <c r="I53" s="44"/>
-      <c r="J53" s="45">
-        <v>6</v>
-      </c>
-      <c r="K53" s="45"/>
+      <c r="B53" s="55"/>
+      <c r="C53" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="D53" s="56">
+        <v>8</v>
+      </c>
+      <c r="E53" s="56">
+        <v>8</v>
+      </c>
+      <c r="F53" s="57">
+        <v>8</v>
+      </c>
+      <c r="G53" s="57">
+        <v>8</v>
+      </c>
+      <c r="H53" s="58">
+        <v>8</v>
+      </c>
+      <c r="I53" s="58">
+        <v>8</v>
+      </c>
+      <c r="J53" s="59">
+        <v>8</v>
+      </c>
+      <c r="K53" s="59">
+        <v>8</v>
+      </c>
     </row>
     <row r="54" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="33"/>
-      <c r="B54" s="69"/>
-      <c r="C54" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D54" s="65">
+      <c r="A54" s="91"/>
+      <c r="B54" s="96"/>
+      <c r="C54" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D54" s="92">
+        <v>4</v>
+      </c>
+      <c r="E54" s="92">
+        <v>4</v>
+      </c>
+      <c r="F54" s="93">
+        <v>4</v>
+      </c>
+      <c r="G54" s="93">
+        <v>4</v>
+      </c>
+      <c r="H54" s="94">
+        <v>4</v>
+      </c>
+      <c r="I54" s="94">
+        <v>4</v>
+      </c>
+      <c r="J54" s="95">
+        <v>4</v>
+      </c>
+      <c r="K54" s="95">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="33"/>
+      <c r="B55" s="66"/>
+      <c r="C55" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D55" s="62">
         <v>2</v>
       </c>
-      <c r="E54" s="65"/>
-      <c r="F54" s="66">
+      <c r="E55" s="62">
         <v>2</v>
       </c>
-      <c r="G54" s="66"/>
-      <c r="H54" s="67">
+      <c r="F55" s="63">
         <v>2</v>
       </c>
-      <c r="I54" s="67"/>
-      <c r="J54" s="68">
+      <c r="G55" s="63">
         <v>2</v>
       </c>
-      <c r="K54" s="68"/>
-    </row>
-    <row r="55" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4"/>
-      <c r="C55" s="5" t="s">
+      <c r="H55" s="64">
+        <v>2</v>
+      </c>
+      <c r="I55" s="64">
+        <v>2</v>
+      </c>
+      <c r="J55" s="65">
+        <v>2</v>
+      </c>
+      <c r="K55" s="65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D55" s="46">
-        <f>SUM(D24:D54)</f>
-        <v>52</v>
-      </c>
-      <c r="E55" s="46">
-        <f>SUM(E24:E54)</f>
-        <v>0</v>
-      </c>
-      <c r="F55" s="46">
-        <f>SUM(F24:F54)</f>
+      <c r="D56" s="46">
+        <f t="shared" ref="D56:K56" si="0">SUM(D24:D55)</f>
+        <v>55</v>
+      </c>
+      <c r="E56" s="46">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="F56" s="46">
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="G55" s="46">
-        <f>SUM(G24:G54)</f>
-        <v>0</v>
-      </c>
-      <c r="H55" s="46">
-        <f>SUM(H24:H54)</f>
-        <v>52</v>
-      </c>
-      <c r="I55" s="46">
-        <f>SUM(I24:I54)</f>
-        <v>0</v>
-      </c>
-      <c r="J55" s="46">
-        <f>SUM(J24:J54)</f>
-        <v>48</v>
-      </c>
-      <c r="K55" s="46">
-        <f>SUM(K24:K54)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="47"/>
-      <c r="E56" s="47"/>
-      <c r="F56" s="47"/>
-      <c r="G56" s="47"/>
-      <c r="H56" s="47"/>
-      <c r="I56" s="47"/>
-      <c r="J56" s="47"/>
-      <c r="K56" s="47"/>
+      <c r="G56" s="46">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="H56" s="46">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="I56" s="46">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="J56" s="46">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="K56" s="46">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
     </row>
     <row r="57" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="9"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="11" t="s">
+      <c r="A57" s="8"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47"/>
+      <c r="F57" s="47"/>
+      <c r="G57" s="47"/>
+      <c r="H57" s="47"/>
+      <c r="I57" s="47"/>
+      <c r="J57" s="47"/>
+      <c r="K57" s="47"/>
+    </row>
+    <row r="58" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="9"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D57" s="48">
-        <f>SUM(D55,D23,)</f>
+      <c r="D58" s="48">
+        <f>SUM(D56,D23,)</f>
+        <v>77</v>
+      </c>
+      <c r="E58" s="48">
+        <f>SUM(E56,E23,)</f>
+        <v>119</v>
+      </c>
+      <c r="F58" s="49">
+        <f>SUM(F56,F23,)</f>
         <v>74</v>
       </c>
-      <c r="E57" s="48">
-        <f>SUM(E55,E23,)</f>
-        <v>27</v>
-      </c>
-      <c r="F57" s="49">
-        <f>SUM(F55,F23,)</f>
-        <v>74</v>
-      </c>
-      <c r="G57" s="49">
-        <f>SUM(G55,G23,)</f>
-        <v>23</v>
-      </c>
-      <c r="H57" s="50">
-        <f>SUM(H55,H23,)</f>
-        <v>71</v>
-      </c>
-      <c r="I57" s="50">
-        <f>SUM(I55,I23,)</f>
-        <v>23</v>
-      </c>
-      <c r="J57" s="51">
-        <f>SUM(J55,J23,)</f>
-        <v>70</v>
-      </c>
-      <c r="K57" s="51">
-        <f>SUM(K55,K23,)</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="12"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="86">
-        <f t="shared" ref="D58" si="0">SUM(80-D57)</f>
-        <v>6</v>
-      </c>
-      <c r="E58" s="86">
-        <f t="shared" ref="E58" si="1">SUM(80-E57)</f>
-        <v>53</v>
-      </c>
-      <c r="F58" s="86">
-        <f t="shared" ref="F58" si="2">SUM(80-F57)</f>
-        <v>6</v>
-      </c>
-      <c r="G58" s="86">
-        <f t="shared" ref="G58" si="3">SUM(80-G57)</f>
-        <v>57</v>
-      </c>
-      <c r="H58" s="86">
-        <f t="shared" ref="H58" si="4">SUM(80-H57)</f>
-        <v>9</v>
-      </c>
-      <c r="I58" s="86">
-        <f t="shared" ref="I58" si="5">SUM(80-I57)</f>
-        <v>57</v>
-      </c>
-      <c r="J58" s="86">
-        <f t="shared" ref="J58" si="6">SUM(80-J57)</f>
-        <v>10</v>
-      </c>
-      <c r="K58" s="86">
-        <f t="shared" ref="K58" si="7">SUM(80-K57)</f>
-        <v>56</v>
+      <c r="G58" s="49">
+        <f>SUM(G56,G23,)</f>
+        <v>107</v>
+      </c>
+      <c r="H58" s="50">
+        <f>SUM(H56,H23,)</f>
+        <v>75</v>
+      </c>
+      <c r="I58" s="50">
+        <f>SUM(I56,I23,)</f>
+        <v>105</v>
+      </c>
+      <c r="J58" s="51">
+        <f>SUM(J56,J23,)</f>
+        <v>75</v>
+      </c>
+      <c r="K58" s="51">
+        <f>SUM(K56,K23,)</f>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="12"/>
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
-      <c r="H59" s="12"/>
-      <c r="I59" s="12"/>
-      <c r="J59" s="12"/>
-      <c r="K59" s="12"/>
-    </row>
-    <row r="60" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12"/>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="12"/>
-      <c r="I61" s="12"/>
-      <c r="J61" s="12"/>
-      <c r="K61" s="12"/>
-    </row>
+      <c r="D59" s="83"/>
+      <c r="E59" s="83"/>
+      <c r="F59" s="83"/>
+      <c r="G59" s="83"/>
+      <c r="H59" s="83"/>
+      <c r="I59" s="83"/>
+      <c r="J59" s="83"/>
+      <c r="K59" s="83"/>
+    </row>
+    <row r="60" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="12"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="12"/>
+      <c r="K60" s="12"/>
+    </row>
+    <row r="61" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="62" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="12"/>
       <c r="B62" s="12"/>
@@ -6470,6 +7169,19 @@
       <c r="I136" s="12"/>
       <c r="J136" s="12"/>
       <c r="K136" s="12"/>
+    </row>
+    <row r="137" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="12"/>
+      <c r="B137" s="12"/>
+      <c r="C137" s="12"/>
+      <c r="D137" s="12"/>
+      <c r="E137" s="12"/>
+      <c r="F137" s="12"/>
+      <c r="G137" s="12"/>
+      <c r="H137" s="12"/>
+      <c r="I137" s="12"/>
+      <c r="J137" s="12"/>
+      <c r="K137" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6520,13 +7232,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Volgorde_x0020_Documenten xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">9999</Volgorde_x0020_Documenten>
-    <Categorie xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Extra</Categorie>
-    <Week xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Geen week</Week>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6691,20 +7402,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Volgorde_x0020_Documenten xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">9999</Volgorde_x0020_Documenten>
+    <Categorie xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Extra</Categorie>
+    <Week xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Geen week</Week>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29FDA2D9-0F29-4761-875B-F7795DA98BB3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DD477B0-7FDC-4B12-8DED-561A832309BE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6728,9 +7438,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DD477B0-7FDC-4B12-8DED-561A832309BE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29FDA2D9-0F29-4761-875B-F7795DA98BB3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>